<commit_message>
files from zaid added, more alpha div modeling post epi meeting
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="19900" windowHeight="14200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="4660" yWindow="0" windowWidth="19900" windowHeight="14200" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="RIchness" sheetId="3" r:id="rId3"/>
     <sheet name="plotting" sheetId="4" r:id="rId4"/>
     <sheet name="reports" sheetId="5" r:id="rId5"/>
+    <sheet name="Table_1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -173,13 +174,115 @@
   </si>
   <si>
     <t>Nval</t>
+  </si>
+  <si>
+    <t>No O157</t>
+  </si>
+  <si>
+    <t>EHEC/aEPEC</t>
+  </si>
+  <si>
+    <t>Day 1 (%)</t>
+  </si>
+  <si>
+    <t>Day 2 (%)</t>
+  </si>
+  <si>
+    <t>Day 3 (%)</t>
+  </si>
+  <si>
+    <t>Day 4 (%)</t>
+  </si>
+  <si>
+    <t>Day 5 (%)</t>
+  </si>
+  <si>
+    <t>Farm 1</t>
+  </si>
+  <si>
+    <t>Farm 2</t>
+  </si>
+  <si>
+    <t>Ever Shed</t>
+  </si>
+  <si>
+    <t>By Sample</t>
+  </si>
+  <si>
+    <t>By Cow</t>
+  </si>
+  <si>
+    <t>9 (45)</t>
+  </si>
+  <si>
+    <t>11 (55)</t>
+  </si>
+  <si>
+    <t>7 (35)</t>
+  </si>
+  <si>
+    <t>13 (65)</t>
+  </si>
+  <si>
+    <t>4 (20)</t>
+  </si>
+  <si>
+    <t>5 (25)</t>
+  </si>
+  <si>
+    <t>0 (0)</t>
+  </si>
+  <si>
+    <t>18 (90)</t>
+  </si>
+  <si>
+    <t>19 (95)</t>
+  </si>
+  <si>
+    <t>20 (100)</t>
+  </si>
+  <si>
+    <t>17 (85)</t>
+  </si>
+  <si>
+    <t>15 (75)</t>
+  </si>
+  <si>
+    <t>16 (80)</t>
+  </si>
+  <si>
+    <t>2 (10)</t>
+  </si>
+  <si>
+    <t>1 (5)</t>
+  </si>
+  <si>
+    <t>3 (15)</t>
+  </si>
+  <si>
+    <t>All Days (%)</t>
+  </si>
+  <si>
+    <t>84 (84)</t>
+  </si>
+  <si>
+    <t>16 (16)</t>
+  </si>
+  <si>
+    <t>93 (93)</t>
+  </si>
+  <si>
+    <t>7 (7)</t>
+  </si>
+  <si>
+    <t>Table 1: Distribution of O157 shedding metrics in 40 early lactation dairy cattle sampled for 5 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -247,6 +350,32 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -490,7 +619,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -564,8 +693,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -573,23 +742,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -598,18 +755,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -646,6 +858,26 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -682,6 +914,26 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2100,7 +2352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -2683,656 +2935,1033 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
     </row>
     <row r="3" spans="1:18">
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:18">
-      <c r="B4" s="9"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="15" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
     </row>
     <row r="5" spans="1:18">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="18"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="18"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="18"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="9"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="18"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="14"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="18"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="9"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="18"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="14"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="8"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="9"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="9"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="C2:Q2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:A8"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" s="30" customFormat="1" ht="18">
+      <c r="A2" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+    </row>
+    <row r="3" spans="1:10" s="30" customFormat="1" ht="18">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="31"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="35"/>
+      <c r="E15" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="32"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="30"/>
+      <c r="C21" s="35"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22" s="30"/>
+      <c r="C22" s="35"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="B23" s="30"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="B24" s="30"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="B25" s="30"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" s="30"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" s="30"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="30"/>
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="30"/>
+      <c r="C29" s="35"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="30"/>
+      <c r="C30" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
new alpha div modeling with potential confounders
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="0" windowWidth="19900" windowHeight="14200" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="12560" yWindow="0" windowWidth="14420" windowHeight="14060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="85">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Table 1: Distribution of O157 shedding metrics in 40 early lactation dairy cattle sampled for 5 days</t>
+  </si>
+  <si>
+    <t>OTUs</t>
   </si>
 </sst>
 </file>
@@ -619,8 +622,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -759,24 +788,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -817,11 +828,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -878,6 +907,19 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -934,6 +976,19 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2350,10 +2405,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2434,7 +2489,7 @@
         <v>23</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G22" si="0">E3/(SQRT(F3))</f>
+        <f t="shared" ref="G3:G30" si="0">E3/(SQRT(F3))</f>
         <v>6.4977616182969539E-3</v>
       </c>
     </row>
@@ -2892,6 +2947,174 @@
       <c r="G22">
         <f t="shared" si="0"/>
         <v>4.2508734874648582E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>38087.24</v>
+      </c>
+      <c r="E24">
+        <v>1278.33</v>
+      </c>
+      <c r="F24">
+        <v>173</v>
+      </c>
+      <c r="G24">
+        <f>E24/(SQRT(F24))</f>
+        <v>97.189630173670267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25">
+        <v>36472.870000000003</v>
+      </c>
+      <c r="E25">
+        <v>18674.28</v>
+      </c>
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3893.85655213775</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>37923.32</v>
+      </c>
+      <c r="E26">
+        <v>10238.08</v>
+      </c>
+      <c r="F26">
+        <v>117</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>946.51083082826551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27">
+        <v>40093.730000000003</v>
+      </c>
+      <c r="E27">
+        <v>18751.060000000001</v>
+      </c>
+      <c r="F27">
+        <v>59</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2441.1800811360877</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28">
+        <v>31270.55</v>
+      </c>
+      <c r="E28">
+        <v>10556.13</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2360.4224259324851</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>37923.32</v>
+      </c>
+      <c r="E29">
+        <v>10238.08</v>
+      </c>
+      <c r="F29">
+        <v>117</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>946.51083082826551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30">
+        <v>37860.01</v>
+      </c>
+      <c r="E30">
+        <v>17421.23</v>
+      </c>
+      <c r="F30">
+        <v>79</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1960.0415092249475</v>
       </c>
     </row>
   </sheetData>
@@ -2935,23 +3158,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="7"/>
@@ -2973,27 +3196,27 @@
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="7"/>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27" t="s">
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="7"/>
@@ -3044,10 +3267,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -3065,7 +3288,7 @@
       <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="49" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -3088,7 +3311,7 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="25"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
@@ -3128,7 +3351,7 @@
       <c r="Q9" s="14"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="49" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3151,7 +3374,7 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="25"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
@@ -3191,7 +3414,7 @@
       <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="49" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -3215,7 +3438,7 @@
       <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="24"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
@@ -3600,7 +3823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -3614,107 +3837,107 @@
     <col min="6" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="30" customFormat="1" ht="18">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:10" s="24" customFormat="1" ht="18">
+      <c r="A2" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-    </row>
-    <row r="3" spans="1:10" s="30" customFormat="1" ht="18">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+    </row>
+    <row r="3" spans="1:10" s="24" customFormat="1" ht="18">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="29" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="29" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3722,154 +3945,154 @@
       <c r="A8" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="30"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="J10" s="31"/>
+      <c r="J10" s="25"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="J11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="43" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="43" t="s">
+      <c r="D12" s="37"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="J12" s="31"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="H13" s="32"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="42" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="32"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="42" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="32"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="42" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="32"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -3877,87 +4100,87 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="29" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="29" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="48"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="49" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="50" t="s">
+      <c r="F20" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="30"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="30"/>
-      <c r="C22" s="35"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="30"/>
+      <c r="B23" s="24"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="30"/>
+      <c r="B24" s="24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="30"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="30"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="30"/>
+      <c r="B27" s="24"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="30"/>
-      <c r="C28" s="35"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="30"/>
-      <c r="C29" s="35"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="30"/>
-      <c r="C30" s="35"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
more alpha div associations and box and whisker plot
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="0" windowWidth="14420" windowHeight="14060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
     <sheet name="Shannons" sheetId="2" r:id="rId2"/>
     <sheet name="RIchness" sheetId="3" r:id="rId3"/>
-    <sheet name="plotting" sheetId="4" r:id="rId4"/>
-    <sheet name="reports" sheetId="5" r:id="rId5"/>
-    <sheet name="Table_1" sheetId="6" r:id="rId6"/>
+    <sheet name="reports" sheetId="5" r:id="rId4"/>
+    <sheet name="Table_1" sheetId="6" r:id="rId5"/>
+    <sheet name="plotting" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="99">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -279,6 +280,48 @@
   </si>
   <si>
     <t>OTUs</t>
+  </si>
+  <si>
+    <t>Alphadiv</t>
+  </si>
+  <si>
+    <t>O157metric</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC</t>
+  </si>
+  <si>
+    <t>Evnev</t>
+  </si>
+  <si>
+    <t>Never shed</t>
+  </si>
+  <si>
+    <t>Intermittent</t>
+  </si>
+  <si>
+    <t>Multi-day</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>upper</t>
+  </si>
+  <si>
+    <t>ymin</t>
+  </si>
+  <si>
+    <t>ymax</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Shed</t>
   </si>
 </sst>
 </file>
@@ -622,8 +665,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -850,7 +905,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -920,6 +975,12 @@
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -989,6 +1050,12 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2405,731 +2472,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2">
-        <v>0.73775679999999999</v>
-      </c>
-      <c r="E2">
-        <v>2.944107E-2</v>
-      </c>
-      <c r="F2">
-        <v>173</v>
-      </c>
-      <c r="G2">
-        <f>E2/(SQRT(F2))</f>
-        <v>2.2383631028115888E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>0.74294559999999998</v>
-      </c>
-      <c r="E3">
-        <v>3.1162169999999999E-2</v>
-      </c>
-      <c r="F3">
-        <v>23</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G30" si="0">E3/(SQRT(F3))</f>
-        <v>6.4977616182969539E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>0.73676620000000004</v>
-      </c>
-      <c r="E4">
-        <v>3.0212180000000002E-2</v>
-      </c>
-      <c r="F4">
-        <v>117</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>2.7931170290653238E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5">
-        <v>0.73792630000000003</v>
-      </c>
-      <c r="E5">
-        <v>2.5476809999999999E-2</v>
-      </c>
-      <c r="F5">
-        <v>59</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>3.3167981491653634E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6">
-        <v>0.74901879999999998</v>
-      </c>
-      <c r="E6">
-        <v>3.6192099999999998E-2</v>
-      </c>
-      <c r="F6">
-        <v>20</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>8.0927995848470123E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7">
-        <v>0.73676620000000004</v>
-      </c>
-      <c r="E7">
-        <v>3.0212180000000002E-2</v>
-      </c>
-      <c r="F7">
-        <v>117</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>2.7931170290653238E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>0.74073449999999996</v>
-      </c>
-      <c r="E8">
-        <v>2.8727570000000001E-2</v>
-      </c>
-      <c r="F8">
-        <v>79</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>3.2321041430005419E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9">
-        <v>4184.04</v>
-      </c>
-      <c r="E9">
-        <v>1132.05</v>
-      </c>
-      <c r="F9">
-        <v>173</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>86.068167717337005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10">
-        <v>4126.174</v>
-      </c>
-      <c r="E10">
-        <v>1725.664</v>
-      </c>
-      <c r="F10">
-        <v>23</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>359.82581781938791</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>4206.3249999999998</v>
-      </c>
-      <c r="E11">
-        <v>964.70799999999997</v>
-      </c>
-      <c r="F11">
-        <v>117</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>89.187286150008049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12">
-        <v>4250.3900000000003</v>
-      </c>
-      <c r="E12">
-        <v>1557.9690000000001</v>
-      </c>
-      <c r="F12">
-        <v>59</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>202.83028745188321</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13">
-        <v>3791.4</v>
-      </c>
-      <c r="E13">
-        <v>1335.271</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>298.57567243841214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14">
-        <v>4206.3249999999998</v>
-      </c>
-      <c r="E14">
-        <v>964.70799999999997</v>
-      </c>
-      <c r="F14">
-        <v>117</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>89.187286150008049</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15">
-        <v>4134.1899999999996</v>
-      </c>
-      <c r="E15">
-        <v>1509.8150000000001</v>
-      </c>
-      <c r="F15">
-        <v>79</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>169.86745891366249</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16">
-        <v>6.1123589999999997</v>
-      </c>
-      <c r="E16">
-        <v>0.32952680000000001</v>
-      </c>
-      <c r="F16">
-        <v>173</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>2.5053458672105799E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>6.1234979999999997</v>
-      </c>
-      <c r="E17">
-        <v>0.40001009999999998</v>
-      </c>
-      <c r="F17">
-        <v>23</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
-        <v>8.3407871618411886E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18">
-        <v>6.1219640000000002</v>
-      </c>
-      <c r="E18">
-        <v>0.30857210000000002</v>
-      </c>
-      <c r="F18">
-        <v>117</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="0"/>
-        <v>2.852750073660517E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19">
-        <v>6.0983749999999999</v>
-      </c>
-      <c r="E19">
-        <v>0.30313040000000002</v>
-      </c>
-      <c r="F19">
-        <v>59</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>3.9464216661181536E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20">
-        <v>6.1102359999999996</v>
-      </c>
-      <c r="E20">
-        <v>0.55265310000000001</v>
-      </c>
-      <c r="F20">
-        <v>20</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="0"/>
-        <v>0.1235769899575989</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21">
-        <v>6.1219640000000002</v>
-      </c>
-      <c r="E21">
-        <v>0.30857210000000002</v>
-      </c>
-      <c r="F21">
-        <v>117</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>2.852750073660517E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22">
-        <v>6.1013780000000004</v>
-      </c>
-      <c r="E22">
-        <v>0.37782589999999999</v>
-      </c>
-      <c r="F22">
-        <v>79</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="0"/>
-        <v>4.2508734874648582E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24">
-        <v>38087.24</v>
-      </c>
-      <c r="E24">
-        <v>1278.33</v>
-      </c>
-      <c r="F24">
-        <v>173</v>
-      </c>
-      <c r="G24">
-        <f>E24/(SQRT(F24))</f>
-        <v>97.189630173670267</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25">
-        <v>36472.870000000003</v>
-      </c>
-      <c r="E25">
-        <v>18674.28</v>
-      </c>
-      <c r="F25">
-        <v>23</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>3893.85655213775</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26">
-        <v>37923.32</v>
-      </c>
-      <c r="E26">
-        <v>10238.08</v>
-      </c>
-      <c r="F26">
-        <v>117</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="0"/>
-        <v>946.51083082826551</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27">
-        <v>40093.730000000003</v>
-      </c>
-      <c r="E27">
-        <v>18751.060000000001</v>
-      </c>
-      <c r="F27">
-        <v>59</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>2441.1800811360877</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28">
-        <v>31270.55</v>
-      </c>
-      <c r="E28">
-        <v>10556.13</v>
-      </c>
-      <c r="F28">
-        <v>20</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>2360.4224259324851</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29">
-        <v>37923.32</v>
-      </c>
-      <c r="E29">
-        <v>10238.08</v>
-      </c>
-      <c r="F29">
-        <v>117</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="0"/>
-        <v>946.51083082826551</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30">
-        <v>37860.01</v>
-      </c>
-      <c r="E30">
-        <v>17421.23</v>
-      </c>
-      <c r="F30">
-        <v>79</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="0"/>
-        <v>1960.0415092249475</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
@@ -3819,7 +3161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J30"/>
   <sheetViews>
@@ -4194,4 +3536,1322 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>0.73775679999999999</v>
+      </c>
+      <c r="E2">
+        <v>2.944107E-2</v>
+      </c>
+      <c r="F2">
+        <v>173</v>
+      </c>
+      <c r="G2">
+        <f>E2/(SQRT(F2))</f>
+        <v>2.2383631028115888E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>0.74294559999999998</v>
+      </c>
+      <c r="E3">
+        <v>3.1162169999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>23</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G30" si="0">E3/(SQRT(F3))</f>
+        <v>6.4977616182969539E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>0.73676620000000004</v>
+      </c>
+      <c r="E4">
+        <v>3.0212180000000002E-2</v>
+      </c>
+      <c r="F4">
+        <v>117</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2.7931170290653238E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>0.73792630000000003</v>
+      </c>
+      <c r="E5">
+        <v>2.5476809999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>3.3167981491653634E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>0.74901879999999998</v>
+      </c>
+      <c r="E6">
+        <v>3.6192099999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>8.0927995848470123E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0.73676620000000004</v>
+      </c>
+      <c r="E7">
+        <v>3.0212180000000002E-2</v>
+      </c>
+      <c r="F7">
+        <v>117</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2.7931170290653238E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>0.74073449999999996</v>
+      </c>
+      <c r="E8">
+        <v>2.8727570000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>79</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3.2321041430005419E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>4184.04</v>
+      </c>
+      <c r="E9">
+        <v>1132.05</v>
+      </c>
+      <c r="F9">
+        <v>173</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>86.068167717337005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>4126.174</v>
+      </c>
+      <c r="E10">
+        <v>1725.664</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>359.82581781938791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>4206.3249999999998</v>
+      </c>
+      <c r="E11">
+        <v>964.70799999999997</v>
+      </c>
+      <c r="F11">
+        <v>117</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>89.187286150008049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>4250.3900000000003</v>
+      </c>
+      <c r="E12">
+        <v>1557.9690000000001</v>
+      </c>
+      <c r="F12">
+        <v>59</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>202.83028745188321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13">
+        <v>3791.4</v>
+      </c>
+      <c r="E13">
+        <v>1335.271</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>298.57567243841214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>4206.3249999999998</v>
+      </c>
+      <c r="E14">
+        <v>964.70799999999997</v>
+      </c>
+      <c r="F14">
+        <v>117</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>89.187286150008049</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>4134.1899999999996</v>
+      </c>
+      <c r="E15">
+        <v>1509.8150000000001</v>
+      </c>
+      <c r="F15">
+        <v>79</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>169.86745891366249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>6.1123589999999997</v>
+      </c>
+      <c r="E16">
+        <v>0.32952680000000001</v>
+      </c>
+      <c r="F16">
+        <v>173</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>2.5053458672105799E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>6.1234979999999997</v>
+      </c>
+      <c r="E17">
+        <v>0.40001009999999998</v>
+      </c>
+      <c r="F17">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>8.3407871618411886E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>6.1219640000000002</v>
+      </c>
+      <c r="E18">
+        <v>0.30857210000000002</v>
+      </c>
+      <c r="F18">
+        <v>117</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>2.852750073660517E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>6.0983749999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.30313040000000002</v>
+      </c>
+      <c r="F19">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>3.9464216661181536E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>6.1102359999999996</v>
+      </c>
+      <c r="E20">
+        <v>0.55265310000000001</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0.1235769899575989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>6.1219640000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.30857210000000002</v>
+      </c>
+      <c r="F21">
+        <v>117</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>2.852750073660517E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>6.1013780000000004</v>
+      </c>
+      <c r="E22">
+        <v>0.37782589999999999</v>
+      </c>
+      <c r="F22">
+        <v>79</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>4.2508734874648582E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24">
+        <v>38087.24</v>
+      </c>
+      <c r="E24">
+        <v>1278.33</v>
+      </c>
+      <c r="F24">
+        <v>173</v>
+      </c>
+      <c r="G24">
+        <f>E24/(SQRT(F24))</f>
+        <v>97.189630173670267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25">
+        <v>36472.870000000003</v>
+      </c>
+      <c r="E25">
+        <v>18674.28</v>
+      </c>
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3893.85655213775</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>37923.32</v>
+      </c>
+      <c r="E26">
+        <v>10238.08</v>
+      </c>
+      <c r="F26">
+        <v>117</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>946.51083082826551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27">
+        <v>40093.730000000003</v>
+      </c>
+      <c r="E27">
+        <v>18751.060000000001</v>
+      </c>
+      <c r="F27">
+        <v>59</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2441.1800811360877</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28">
+        <v>31270.55</v>
+      </c>
+      <c r="E28">
+        <v>10556.13</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2360.4224259324851</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>37923.32</v>
+      </c>
+      <c r="E29">
+        <v>10238.08</v>
+      </c>
+      <c r="F29">
+        <v>117</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>946.51083082826551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30">
+        <v>37860.01</v>
+      </c>
+      <c r="E30">
+        <v>17421.23</v>
+      </c>
+      <c r="F30">
+        <v>79</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1960.0415092249475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>526</v>
+      </c>
+      <c r="E2">
+        <v>8414</v>
+      </c>
+      <c r="F2">
+        <v>4215</v>
+      </c>
+      <c r="G2">
+        <v>3623</v>
+      </c>
+      <c r="H2">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3">
+        <v>1122</v>
+      </c>
+      <c r="E3">
+        <v>9913</v>
+      </c>
+      <c r="F3">
+        <v>3922</v>
+      </c>
+      <c r="G3">
+        <v>3216</v>
+      </c>
+      <c r="H3">
+        <v>4813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>4.7080000000000002</v>
+      </c>
+      <c r="E4">
+        <v>6.6840000000000002</v>
+      </c>
+      <c r="F4">
+        <v>6.1580000000000004</v>
+      </c>
+      <c r="G4">
+        <v>5.9139999999999997</v>
+      </c>
+      <c r="H4">
+        <v>6.3739999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5">
+        <v>5.351</v>
+      </c>
+      <c r="E5">
+        <v>6.7930000000000001</v>
+      </c>
+      <c r="F5">
+        <v>6.0780000000000003</v>
+      </c>
+      <c r="G5">
+        <v>5.8680000000000003</v>
+      </c>
+      <c r="H5">
+        <v>6.4530000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>0.62958999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.83303000000000005</v>
+      </c>
+      <c r="F6">
+        <v>0.73816000000000004</v>
+      </c>
+      <c r="G6">
+        <v>0.72043999999999997</v>
+      </c>
+      <c r="H6">
+        <v>0.75544999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7">
+        <v>0.68</v>
+      </c>
+      <c r="E7">
+        <v>0.78718999999999995</v>
+      </c>
+      <c r="F7">
+        <v>0.74458000000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.72436999999999996</v>
+      </c>
+      <c r="H7">
+        <v>0.77410000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>3359.8</v>
+      </c>
+      <c r="E8">
+        <v>5180</v>
+      </c>
+      <c r="F8">
+        <v>4025.9</v>
+      </c>
+      <c r="G8">
+        <v>3811.25</v>
+      </c>
+      <c r="H8">
+        <v>4576.1000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9">
+        <v>2440</v>
+      </c>
+      <c r="E9">
+        <v>7644.4</v>
+      </c>
+      <c r="F9">
+        <v>4094.3</v>
+      </c>
+      <c r="G9">
+        <v>3481.75</v>
+      </c>
+      <c r="H9">
+        <v>4409.4799999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>5.7953999999999999</v>
+      </c>
+      <c r="E10">
+        <v>6.4438000000000004</v>
+      </c>
+      <c r="F10">
+        <v>6.1097000000000001</v>
+      </c>
+      <c r="G10">
+        <v>5.9298999999999999</v>
+      </c>
+      <c r="H10">
+        <v>6.3144999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11">
+        <v>5.3346</v>
+      </c>
+      <c r="E11">
+        <v>6.6280000000000001</v>
+      </c>
+      <c r="F11">
+        <v>6.0579999999999998</v>
+      </c>
+      <c r="G11">
+        <v>5.9375</v>
+      </c>
+      <c r="H11">
+        <v>6.2988999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>0.70140000000000002</v>
+      </c>
+      <c r="E12">
+        <v>0.78239000000000003</v>
+      </c>
+      <c r="F12">
+        <v>0.74065000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.71999000000000002</v>
+      </c>
+      <c r="H12">
+        <v>0.75361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>0.69889000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.77873999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.73880999999999997</v>
+      </c>
+      <c r="G13">
+        <v>0.72119</v>
+      </c>
+      <c r="H13">
+        <v>0.76083000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>3359.8</v>
+      </c>
+      <c r="E14">
+        <v>5180</v>
+      </c>
+      <c r="F14">
+        <v>4025.9</v>
+      </c>
+      <c r="G14">
+        <v>3811.25</v>
+      </c>
+      <c r="H14">
+        <v>4576.1000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15">
+        <v>2877.4</v>
+      </c>
+      <c r="E15">
+        <v>7644.4</v>
+      </c>
+      <c r="F15">
+        <v>4106.8</v>
+      </c>
+      <c r="G15">
+        <v>3779.05</v>
+      </c>
+      <c r="H15">
+        <v>4409.4799999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16">
+        <v>2440</v>
+      </c>
+      <c r="E16">
+        <v>5000.3999999999996</v>
+      </c>
+      <c r="F16">
+        <v>3862.6</v>
+      </c>
+      <c r="G16">
+        <v>3234.7</v>
+      </c>
+      <c r="H16">
+        <v>4419.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>5.7949999999999999</v>
+      </c>
+      <c r="E17">
+        <v>6.444</v>
+      </c>
+      <c r="F17">
+        <v>6.1097000000000001</v>
+      </c>
+      <c r="G17">
+        <v>5.9298999999999999</v>
+      </c>
+      <c r="H17">
+        <v>6.3144999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>5.8512000000000004</v>
+      </c>
+      <c r="E18">
+        <v>6.5640000000000001</v>
+      </c>
+      <c r="F18">
+        <v>6.0585000000000004</v>
+      </c>
+      <c r="G18">
+        <v>5.9375</v>
+      </c>
+      <c r="H18">
+        <v>6.2115999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>5.3346</v>
+      </c>
+      <c r="E19">
+        <v>6.6280000000000001</v>
+      </c>
+      <c r="F19">
+        <v>6.2392000000000003</v>
+      </c>
+      <c r="G19">
+        <v>5.8475999999999999</v>
+      </c>
+      <c r="H19">
+        <v>6.5018000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20">
+        <v>0.70142000000000004</v>
+      </c>
+      <c r="E20">
+        <v>0.78239000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.74065000000000003</v>
+      </c>
+      <c r="G20">
+        <v>0.71999000000000002</v>
+      </c>
+      <c r="H20">
+        <v>0.75361</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21">
+        <v>0.70843</v>
+      </c>
+      <c r="E21">
+        <v>0.76997000000000004</v>
+      </c>
+      <c r="F21">
+        <v>0.73543000000000003</v>
+      </c>
+      <c r="G21">
+        <v>0.72119</v>
+      </c>
+      <c r="H21">
+        <v>0.75231000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22">
+        <v>0.69889000000000001</v>
+      </c>
+      <c r="E22">
+        <v>0.77873999999999999</v>
+      </c>
+      <c r="F22">
+        <v>0.75922000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.73126999999999998</v>
+      </c>
+      <c r="H22">
+        <v>0.77697000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made final r scripts with all relevant epi modeling and differential abundance testing code. for purposes of the manuscript being written 6.5.17
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="380" yWindow="80" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>aEPEC/EHEC</t>
-  </si>
-  <si>
-    <t>Evnev</t>
-  </si>
-  <si>
     <t>Never shed</t>
   </si>
   <si>
@@ -321,7 +315,32 @@
     <t>median</t>
   </si>
   <si>
-    <t>Shed</t>
+    <t>O157</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Shed </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 time</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -665,8 +684,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="151">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -905,7 +928,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="151">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -981,6 +1004,8 @@
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1056,6 +1081,8 @@
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4268,10 +4295,14 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -4284,19 +4315,19 @@
         <v>87</v>
       </c>
       <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
         <v>95</v>
       </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>97</v>
-      </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4333,7 +4364,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>1122</v>
@@ -4385,7 +4416,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>5.351</v>
@@ -4437,7 +4468,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D7">
         <v>0.68</v>
@@ -4460,10 +4491,10 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>3359.8</v>
@@ -4486,10 +4517,10 @@
         <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9">
         <v>2440</v>
@@ -4512,10 +4543,10 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10">
         <v>5.7953999999999999</v>
@@ -4538,10 +4569,10 @@
         <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11">
         <v>5.3346</v>
@@ -4564,10 +4595,10 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D12">
         <v>0.70140000000000002</v>
@@ -4590,10 +4621,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13">
         <v>0.69889000000000001</v>
@@ -4619,7 +4650,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14">
         <v>3359.8</v>
@@ -4645,7 +4676,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D15">
         <v>2877.4</v>
@@ -4671,7 +4702,7 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D16">
         <v>2440</v>
@@ -4697,7 +4728,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D17">
         <v>5.7949999999999999</v>
@@ -4723,7 +4754,7 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18">
         <v>5.8512000000000004</v>
@@ -4749,7 +4780,7 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <v>5.3346</v>
@@ -4775,7 +4806,7 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20">
         <v>0.70142000000000004</v>
@@ -4801,7 +4832,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21">
         <v>0.70843</v>
@@ -4827,7 +4858,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22">
         <v>0.69889000000000001</v>

</xml_diff>

<commit_message>
updated final diff abundane and also made diff abundance plot
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="80" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12140" windowHeight="13420" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Table_1" sheetId="6" r:id="rId5"/>
     <sheet name="plotting" sheetId="4" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="Diff abund" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="126">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -342,12 +343,144 @@
       <t xml:space="preserve"> 1 time</t>
     </r>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>LogFC</t>
+  </si>
+  <si>
+    <t>CI.L</t>
+  </si>
+  <si>
+    <t>CI.R</t>
+  </si>
+  <si>
+    <t>Padj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s__coagulans     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s__producta      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s__neonatale     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f__Acetobacteraceae     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f__Corynebacteriaceae   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f__Pirellulaceae       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">g__Moryella              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">g__Faecalibacterium      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">g__Methanosphaera        </t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Bacillus coagulans</t>
+  </si>
+  <si>
+    <t>Blautia producta</t>
+  </si>
+  <si>
+    <t>Clostridium neonatale</t>
+  </si>
+  <si>
+    <t>Family Acetobacteraceae</t>
+  </si>
+  <si>
+    <t>Family Corynebacteriaceae</t>
+  </si>
+  <si>
+    <t>Family Pirellulaceae</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t>Moryella</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t xml:space="preserve"> spp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t>Faecalibacterium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t xml:space="preserve"> spp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t>Methanosphaera</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+      </rPr>
+      <t xml:space="preserve"> spp</t>
+    </r>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +573,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="4">
@@ -841,7 +985,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -925,6 +1069,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4294,7 +4450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -4885,4 +5041,259 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="53"/>
+    <col min="2" max="2" width="21.83203125" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="53" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="55">
+        <v>0.30889443999999999</v>
+      </c>
+      <c r="E3" s="55">
+        <v>9.4338368000000006E-2</v>
+      </c>
+      <c r="F3" s="55">
+        <v>0.52345050000000004</v>
+      </c>
+      <c r="G3" s="55">
+        <v>9.2291680000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0.13164651999999999</v>
+      </c>
+      <c r="E4" s="55">
+        <v>4.3900270000000003E-3</v>
+      </c>
+      <c r="F4" s="55">
+        <v>0.25890299999999999</v>
+      </c>
+      <c r="G4" s="55">
+        <v>0.36469354999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="55">
+        <v>0.22334511000000001</v>
+      </c>
+      <c r="E5" s="55">
+        <v>-6.7775206000000005E-2</v>
+      </c>
+      <c r="F5" s="55">
+        <v>0.51446539999999996</v>
+      </c>
+      <c r="G5" s="55">
+        <v>0.73922427000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="55">
+        <v>-0.37495079999999997</v>
+      </c>
+      <c r="E6" s="55">
+        <v>-0.57696647000000001</v>
+      </c>
+      <c r="F6" s="55">
+        <v>-0.172935177</v>
+      </c>
+      <c r="G6" s="55">
+        <v>3.9258340000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="55">
+        <v>-0.26487500000000003</v>
+      </c>
+      <c r="E7" s="55">
+        <v>-0.53347986000000003</v>
+      </c>
+      <c r="F7" s="55">
+        <v>3.7298560000000001E-3</v>
+      </c>
+      <c r="G7" s="55">
+        <v>0.96250391000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="55">
+        <v>-0.37401079999999998</v>
+      </c>
+      <c r="E8" s="55">
+        <v>-0.73596147999999995</v>
+      </c>
+      <c r="F8" s="55">
+        <v>-1.2060128999999999E-2</v>
+      </c>
+      <c r="G8" s="55">
+        <v>0.96250391000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="55">
+        <v>0.40642020000000001</v>
+      </c>
+      <c r="E9" s="55">
+        <v>5.9096373000000001E-2</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.75374392999999995</v>
+      </c>
+      <c r="G9" s="55">
+        <v>0.98857209999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="55">
+        <v>0.35030090000000003</v>
+      </c>
+      <c r="E10" s="55">
+        <v>-1.7922747999999999E-2</v>
+      </c>
+      <c r="F10" s="55">
+        <v>0.71852453000000005</v>
+      </c>
+      <c r="G10" s="55">
+        <v>0.98857209999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="55">
+        <v>-0.46468369999999998</v>
+      </c>
+      <c r="E11" s="55">
+        <v>-0.88109932000000002</v>
+      </c>
+      <c r="F11" s="55">
+        <v>-4.8268060000000002E-2</v>
+      </c>
+      <c r="G11" s="55">
+        <v>0.98857209999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed figures a bit and also the contrasts for DESeq2 models
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12140" windowHeight="13420" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="11340" yWindow="180" windowWidth="13200" windowHeight="13300" tabRatio="692" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,8 @@
     <sheet name="Table_1" sheetId="6" r:id="rId5"/>
     <sheet name="plotting" sheetId="4" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
-    <sheet name="Diff abund" sheetId="8" r:id="rId8"/>
+    <sheet name="MGS Diff abund" sheetId="8" r:id="rId8"/>
+    <sheet name="DES Diff abund" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="135">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -474,6 +475,33 @@
   </si>
   <si>
     <t>family</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>s__prausnitzii</t>
+  </si>
+  <si>
+    <t>Faecalibacterium prausnitzii</t>
+  </si>
+  <si>
+    <t>g_Atopobium</t>
+  </si>
+  <si>
+    <t>g_Corynebacterium</t>
+  </si>
+  <si>
+    <t>f_Acetobacteraceae</t>
+  </si>
+  <si>
+    <t>Atopobium spp</t>
+  </si>
+  <si>
+    <t>Corynebacterium spp</t>
+  </si>
+  <si>
+    <t>f_Pirellulaceae</t>
   </si>
 </sst>
 </file>
@@ -828,8 +856,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1050,6 +1082,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1071,20 +1115,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="159">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1162,6 +1194,8 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1239,6 +1273,8 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2657,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R31"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:Q14"/>
+    <sheetView topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2683,23 +2719,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18">
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
     </row>
     <row r="3" spans="1:18">
       <c r="B3" s="7"/>
@@ -2721,27 +2757,27 @@
     </row>
     <row r="4" spans="1:18">
       <c r="B4" s="7"/>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="51" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
+      <c r="Q4" s="55"/>
     </row>
     <row r="5" spans="1:18">
       <c r="B5" s="7"/>
@@ -2792,10 +2828,10 @@
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="48"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -2813,7 +2849,7 @@
       <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="53" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2836,7 +2872,7 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="50"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
@@ -2876,7 +2912,7 @@
       <c r="Q9" s="14"/>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="53" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2899,7 +2935,7 @@
       <c r="Q10" s="14"/>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="50"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="9" t="s">
         <v>25</v>
       </c>
@@ -2939,7 +2975,7 @@
       <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="53" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2963,7 +2999,7 @@
       <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="49"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
@@ -3363,16 +3399,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" s="24" customFormat="1" ht="18">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="1:10" s="24" customFormat="1" ht="18">
       <c r="A3" s="45"/>
@@ -5047,25 +5083,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="53"/>
-    <col min="2" max="2" width="21.83203125" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="53" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="46"/>
+    <col min="2" max="2" width="21.83203125" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="46" t="s">
         <v>122</v>
       </c>
       <c r="D2" t="s">
@@ -5082,214 +5118,406 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="55">
+      <c r="D3" s="48">
         <v>0.30889443999999999</v>
       </c>
-      <c r="E3" s="55">
+      <c r="E3" s="48">
         <v>9.4338368000000006E-2</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="48">
         <v>0.52345050000000004</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="48">
         <v>9.2291680000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="55">
+      <c r="D4" s="48">
         <v>0.13164651999999999</v>
       </c>
-      <c r="E4" s="55">
+      <c r="E4" s="48">
         <v>4.3900270000000003E-3</v>
       </c>
-      <c r="F4" s="55">
+      <c r="F4" s="48">
         <v>0.25890299999999999</v>
       </c>
-      <c r="G4" s="55">
+      <c r="G4" s="48">
         <v>0.36469354999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="55">
+      <c r="D5" s="48">
         <v>0.22334511000000001</v>
       </c>
-      <c r="E5" s="55">
+      <c r="E5" s="48">
         <v>-6.7775206000000005E-2</v>
       </c>
-      <c r="F5" s="55">
+      <c r="F5" s="48">
         <v>0.51446539999999996</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="48">
         <v>0.73922427000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="55">
+      <c r="D6" s="48">
         <v>-0.37495079999999997</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="48">
         <v>-0.57696647000000001</v>
       </c>
-      <c r="F6" s="55">
+      <c r="F6" s="48">
         <v>-0.172935177</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="48">
         <v>3.9258340000000003E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="55">
+      <c r="D7" s="48">
         <v>-0.26487500000000003</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="48">
         <v>-0.53347986000000003</v>
       </c>
-      <c r="F7" s="55">
+      <c r="F7" s="48">
         <v>3.7298560000000001E-3</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="48">
         <v>0.96250391000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="48">
         <v>-0.37401079999999998</v>
       </c>
-      <c r="E8" s="55">
+      <c r="E8" s="48">
         <v>-0.73596147999999995</v>
       </c>
-      <c r="F8" s="55">
+      <c r="F8" s="48">
         <v>-1.2060128999999999E-2</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="48">
         <v>0.96250391000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="48">
         <v>0.40642020000000001</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="48">
         <v>5.9096373000000001E-2</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="48">
         <v>0.75374392999999995</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="48">
         <v>0.98857209999999995</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="48">
         <v>0.35030090000000003</v>
       </c>
-      <c r="E10" s="55">
+      <c r="E10" s="48">
         <v>-1.7922747999999999E-2</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="48">
         <v>0.71852453000000005</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="48">
         <v>0.98857209999999995</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="48">
         <v>-0.46468369999999998</v>
       </c>
-      <c r="E11" s="55">
+      <c r="E11" s="48">
         <v>-0.88109932000000002</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="48">
         <v>-4.8268060000000002E-2</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="48">
         <v>0.98857209999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3">
+        <v>-0.70542199999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.45739999999999997</v>
+      </c>
+      <c r="F3">
+        <f>D3-1.96*E3</f>
+        <v>-1.601926</v>
+      </c>
+      <c r="G3">
+        <f>D3+1.96*E3</f>
+        <v>0.19108199999999997</v>
+      </c>
+      <c r="H3">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4">
+        <v>-0.50427</v>
+      </c>
+      <c r="E4">
+        <v>0.37297000000000002</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F7" si="0">D4-1.96*E4</f>
+        <v>-1.2352912</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G7" si="1">D4+1.96*E4</f>
+        <v>0.22675120000000004</v>
+      </c>
+      <c r="H4">
+        <v>0.97989999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5">
+        <v>0.60281799999999996</v>
+      </c>
+      <c r="E5">
+        <v>0.35009000000000001</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-8.3358400000000055E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1.2889944</v>
+      </c>
+      <c r="H5">
+        <v>0.97989999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6">
+        <v>0.62316329999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.31457000000000002</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>6.6060999999999481E-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1.2397205</v>
+      </c>
+      <c r="H6">
+        <v>0.73760000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>-0.88197000000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.44445000000000001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-1.7530920000000001</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-1.084800000000008E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.73760000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
made dot plots for o157 and diversity tables for manuscript
</commit_message>
<xml_diff>
--- a/excel sheets/Test output for alpha div models.xlsx
+++ b/excel sheets/Test output for alpha div models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="180" windowWidth="13200" windowHeight="13300" tabRatio="692" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10960" windowHeight="13040" tabRatio="692" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Evenness" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,10 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
     <sheet name="MGS Diff abund" sheetId="8" r:id="rId8"/>
     <sheet name="DES Diff abund" sheetId="9" r:id="rId9"/>
+    <sheet name="10" sheetId="10" r:id="rId10"/>
+    <sheet name="11" sheetId="11" r:id="rId11"/>
+    <sheet name="12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet5" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="155">
   <si>
     <t>Pathotype_1</t>
   </si>
@@ -502,6 +506,66 @@
   </si>
   <si>
     <t>f_Pirellulaceae</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Upper_CL</t>
+  </si>
+  <si>
+    <t>Lower_CL</t>
+  </si>
+  <si>
+    <t>Alpha_Diversity</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC vs No O157 1</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC vs No O157 2</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC vs No O157 3</t>
+  </si>
+  <si>
+    <t>Ever shed vs Never shed 1</t>
+  </si>
+  <si>
+    <t>Ever shed vs Never shed 2</t>
+  </si>
+  <si>
+    <t>Ever shed vs Never shed 3</t>
+  </si>
+  <si>
+    <t>Intermittently shed vs Never shed 1</t>
+  </si>
+  <si>
+    <t>Intermittently shed vs Never shed 2</t>
+  </si>
+  <si>
+    <t>Intermittently shed vs Never shed 3</t>
+  </si>
+  <si>
+    <t>Multi-day shed vs Never shed 1</t>
+  </si>
+  <si>
+    <t>Multi-day shed vs Never shed 2</t>
+  </si>
+  <si>
+    <t>Multi-day shed vs Never shed 3</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC 1</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC 2</t>
+  </si>
+  <si>
+    <t>aEPEC/EHEC 3</t>
   </si>
 </sst>
 </file>
@@ -856,8 +920,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1116,7 +1208,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1196,6 +1288,20 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1275,6 +1381,20 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1971,6 +2091,578 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3">
+        <v>0.93</v>
+      </c>
+      <c r="C3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D3">
+        <v>1.54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4">
+        <v>1.04</v>
+      </c>
+      <c r="C4">
+        <v>0.49</v>
+      </c>
+      <c r="D4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5">
+        <v>1.18</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>2.31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3">
+        <v>0.93</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>1.73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>0.36</v>
+      </c>
+      <c r="D4">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5">
+        <v>1.28</v>
+      </c>
+      <c r="C5">
+        <v>0.51</v>
+      </c>
+      <c r="D5">
+        <v>3.24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3">
+        <v>1.06</v>
+      </c>
+      <c r="C3">
+        <v>0.93</v>
+      </c>
+      <c r="D3">
+        <v>1.21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4">
+        <v>0.88</v>
+      </c>
+      <c r="C4">
+        <v>0.32</v>
+      </c>
+      <c r="D4">
+        <v>2.39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5">
+        <v>1.05</v>
+      </c>
+      <c r="C5">
+        <v>0.38</v>
+      </c>
+      <c r="D5">
+        <v>2.92</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6">
+        <v>0.51</v>
+      </c>
+      <c r="C6">
+        <v>0.41</v>
+      </c>
+      <c r="D6">
+        <v>0.64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <v>0.93</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>4.32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.44</v>
+      </c>
+      <c r="D8">
+        <v>11.27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3">
+        <v>0.93</v>
+      </c>
+      <c r="C3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D3">
+        <v>1.54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4">
+        <v>1.04</v>
+      </c>
+      <c r="C4">
+        <v>0.49</v>
+      </c>
+      <c r="D4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5">
+        <v>1.18</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="D5">
+        <v>2.31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6">
+        <v>0.93</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>1.73</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+      <c r="C7">
+        <v>0.36</v>
+      </c>
+      <c r="D7">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8">
+        <v>1.28</v>
+      </c>
+      <c r="C8">
+        <v>0.51</v>
+      </c>
+      <c r="D8">
+        <v>3.24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="35">
+        <v>1.06</v>
+      </c>
+      <c r="C9" s="35">
+        <v>0.93</v>
+      </c>
+      <c r="D9" s="35">
+        <v>1.21</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="35">
+        <v>0.88</v>
+      </c>
+      <c r="C10" s="35">
+        <v>0.32</v>
+      </c>
+      <c r="D10" s="35">
+        <v>2.39</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="35">
+        <v>1.05</v>
+      </c>
+      <c r="C11" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="D11" s="35">
+        <v>2.92</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="35">
+        <v>0.51</v>
+      </c>
+      <c r="C12" s="35">
+        <v>0.41</v>
+      </c>
+      <c r="D12" s="35">
+        <v>0.64</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="35">
+        <v>0.93</v>
+      </c>
+      <c r="C13" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="35">
+        <v>4.32</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="35">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="C14" s="35">
+        <v>0.44</v>
+      </c>
+      <c r="D14" s="35">
+        <v>11.27</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
@@ -5339,7 +6031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>